<commit_message>
Finished Implementation of Algoma Reception Logic
Finished implementation of Algoma reception logic, adding robustness to ensure WebDriver session always closes after upload and adding terminal output to monitor progress of upload.
</commit_message>
<xml_diff>
--- a/Nasco-Database-Web-App/import-manifest.xlsx
+++ b/Nasco-Database-Web-App/import-manifest.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyle.conrad\Documents\PowerShell\AlgomaReception\"/>
     </mc:Choice>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -288,7 +288,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="164">
   <si>
     <t xml:space="preserve">Client inventory </t>
   </si>
@@ -726,6 +726,60 @@
   </si>
   <si>
     <t>9179H5 04</t>
+  </si>
+  <si>
+    <t>Esmark Steel Group - Midwest - 17985</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>TCY0101</t>
+  </si>
+  <si>
+    <t>1798J5 04</t>
+  </si>
+  <si>
+    <t>1200024855 / 2203648 / W237779/2</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>0.0550</t>
+  </si>
+  <si>
+    <t>48.000</t>
+  </si>
+  <si>
+    <t>44,910</t>
+  </si>
+  <si>
+    <t>TCY0103</t>
+  </si>
+  <si>
+    <t>1798J5 05</t>
+  </si>
+  <si>
+    <t>45,040</t>
+  </si>
+  <si>
+    <t>TCY0100</t>
+  </si>
+  <si>
+    <t>1798J5 53</t>
+  </si>
+  <si>
+    <t>44,240</t>
+  </si>
+  <si>
+    <t>TCY0102</t>
+  </si>
+  <si>
+    <t>1798J5 54</t>
+  </si>
+  <si>
+    <t>44,670</t>
   </si>
 </sst>
 </file>
@@ -1281,7 +1335,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E028D80B-E87B-4934-9799-6D8D159AC64A}">
-  <dimension ref="A1:AS7"/>
+  <dimension ref="A1:AS6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="T3" activePane="bottomRight" state="frozen"/>
@@ -1292,41 +1346,41 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1"/>
-    <col min="6" max="6" width="25" customWidth="1"/>
-    <col min="7" max="7" width="28.42578125" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" customWidth="1"/>
-    <col min="17" max="17" width="12.85546875" style="17" customWidth="1"/>
-    <col min="18" max="18" width="14.28515625" customWidth="1"/>
-    <col min="19" max="20" width="10.28515625" customWidth="1"/>
-    <col min="21" max="21" width="15.42578125" customWidth="1"/>
-    <col min="22" max="23" width="10.28515625" customWidth="1"/>
-    <col min="24" max="24" width="14.7109375" customWidth="1"/>
-    <col min="25" max="26" width="10.28515625" customWidth="1"/>
-    <col min="27" max="27" width="15.28515625" customWidth="1"/>
-    <col min="28" max="33" width="10.28515625" customWidth="1"/>
-    <col min="34" max="34" width="11.42578125" customWidth="1"/>
-    <col min="35" max="35" width="12" customWidth="1"/>
-    <col min="36" max="36" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="16.28515625" customWidth="1"/>
-    <col min="41" max="41" width="18.28515625" customWidth="1"/>
-    <col min="42" max="42" width="19.28515625" customWidth="1"/>
-    <col min="43" max="43" width="12.28515625" customWidth="1"/>
-    <col min="44" max="45" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="17" width="12.85546875" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="19" max="20" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="22" max="23" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="25" max="26" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="28" max="33" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="35" max="35" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="40" max="40" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="41" max="41" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="42" max="42" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="43" max="43" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="44" max="45" customWidth="true" width="10.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.25">
@@ -1527,12 +1581,12 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" t="s">
         <v>131</v>
       </c>
       <c r="B3" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="C3" t="s">
         <v>129</v>
@@ -1543,44 +1597,44 @@
       <c r="E3" t="s">
         <v>63</v>
       </c>
-      <c r="F3">
-        <v>1</v>
+      <c r="F3" t="s">
+        <v>147</v>
       </c>
       <c r="G3" t="s">
         <v>83</v>
       </c>
-      <c r="I3">
-        <v>1</v>
+      <c r="I3" t="s">
+        <v>147</v>
       </c>
       <c r="J3" t="s">
         <v>38</v>
       </c>
       <c r="K3" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="L3" t="s">
         <v>57</v>
       </c>
       <c r="M3" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="N3" t="s">
         <v>37</v>
       </c>
       <c r="O3" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="P3" t="s">
         <v>36</v>
       </c>
-      <c r="Q3" s="17" t="s">
-        <v>133</v>
+      <c r="Q3" t="s">
+        <v>151</v>
       </c>
       <c r="R3" t="s">
         <v>42</v>
       </c>
-      <c r="S3">
-        <v>3.9E-2</v>
+      <c r="S3" t="s">
+        <v>152</v>
       </c>
       <c r="T3" t="s">
         <v>46</v>
@@ -1588,14 +1642,14 @@
       <c r="U3" t="s">
         <v>40</v>
       </c>
-      <c r="V3">
-        <v>49.875</v>
+      <c r="V3" t="s">
+        <v>153</v>
       </c>
       <c r="W3" t="s">
         <v>46</v>
       </c>
-      <c r="AF3">
-        <v>37300</v>
+      <c r="AF3" t="s">
+        <v>154</v>
       </c>
       <c r="AG3" t="s">
         <v>49</v>
@@ -1604,12 +1658,12 @@
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" t="s">
         <v>131</v>
       </c>
       <c r="B4" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="C4" t="s">
         <v>129</v>
@@ -1620,44 +1674,44 @@
       <c r="E4" t="s">
         <v>63</v>
       </c>
-      <c r="F4">
-        <v>1</v>
+      <c r="F4" t="s">
+        <v>147</v>
       </c>
       <c r="G4" t="s">
         <v>83</v>
       </c>
-      <c r="I4">
-        <v>1</v>
+      <c r="I4" t="s">
+        <v>147</v>
       </c>
       <c r="J4" t="s">
         <v>38</v>
       </c>
       <c r="K4" t="s">
-        <v>138</v>
+        <v>155</v>
       </c>
       <c r="L4" t="s">
         <v>57</v>
       </c>
       <c r="M4" t="s">
-        <v>139</v>
+        <v>156</v>
       </c>
       <c r="N4" t="s">
         <v>37</v>
       </c>
       <c r="O4" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="P4" t="s">
         <v>36</v>
       </c>
-      <c r="Q4" s="17" t="s">
-        <v>133</v>
+      <c r="Q4" t="s">
+        <v>151</v>
       </c>
       <c r="R4" t="s">
         <v>42</v>
       </c>
-      <c r="S4">
-        <v>3.9E-2</v>
+      <c r="S4" t="s">
+        <v>152</v>
       </c>
       <c r="T4" t="s">
         <v>46</v>
@@ -1665,14 +1719,14 @@
       <c r="U4" t="s">
         <v>40</v>
       </c>
-      <c r="V4">
-        <v>49.875</v>
+      <c r="V4" t="s">
+        <v>153</v>
       </c>
       <c r="W4" t="s">
         <v>46</v>
       </c>
-      <c r="AF4">
-        <v>40380</v>
+      <c r="AF4" t="s">
+        <v>157</v>
       </c>
       <c r="AG4" t="s">
         <v>49</v>
@@ -1681,12 +1735,12 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" t="s">
         <v>131</v>
       </c>
       <c r="B5" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="C5" t="s">
         <v>129</v>
@@ -1697,44 +1751,44 @@
       <c r="E5" t="s">
         <v>63</v>
       </c>
-      <c r="F5">
-        <v>1</v>
+      <c r="F5" t="s">
+        <v>147</v>
       </c>
       <c r="G5" t="s">
         <v>83</v>
       </c>
-      <c r="I5">
-        <v>1</v>
+      <c r="I5" t="s">
+        <v>147</v>
       </c>
       <c r="J5" t="s">
         <v>38</v>
       </c>
       <c r="K5" t="s">
-        <v>140</v>
+        <v>158</v>
       </c>
       <c r="L5" t="s">
         <v>57</v>
       </c>
       <c r="M5" t="s">
-        <v>141</v>
+        <v>159</v>
       </c>
       <c r="N5" t="s">
         <v>37</v>
       </c>
       <c r="O5" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="P5" t="s">
         <v>36</v>
       </c>
-      <c r="Q5" s="17" t="s">
-        <v>133</v>
+      <c r="Q5" t="s">
+        <v>151</v>
       </c>
       <c r="R5" t="s">
         <v>42</v>
       </c>
-      <c r="S5">
-        <v>3.9E-2</v>
+      <c r="S5" t="s">
+        <v>152</v>
       </c>
       <c r="T5" t="s">
         <v>46</v>
@@ -1742,14 +1796,14 @@
       <c r="U5" t="s">
         <v>40</v>
       </c>
-      <c r="V5">
-        <v>49.875</v>
+      <c r="V5" t="s">
+        <v>153</v>
       </c>
       <c r="W5" t="s">
         <v>46</v>
       </c>
-      <c r="AF5">
-        <v>37000</v>
+      <c r="AF5" t="s">
+        <v>160</v>
       </c>
       <c r="AG5" t="s">
         <v>49</v>
@@ -1758,12 +1812,12 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="A6" t="s">
         <v>131</v>
       </c>
       <c r="B6" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="C6" t="s">
         <v>129</v>
@@ -1774,44 +1828,44 @@
       <c r="E6" t="s">
         <v>63</v>
       </c>
-      <c r="F6">
-        <v>1</v>
+      <c r="F6" t="s">
+        <v>147</v>
       </c>
       <c r="G6" t="s">
         <v>83</v>
       </c>
-      <c r="I6">
-        <v>1</v>
+      <c r="I6" t="s">
+        <v>147</v>
       </c>
       <c r="J6" t="s">
         <v>38</v>
       </c>
       <c r="K6" t="s">
-        <v>142</v>
+        <v>161</v>
       </c>
       <c r="L6" t="s">
         <v>57</v>
       </c>
       <c r="M6" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
       <c r="N6" t="s">
         <v>37</v>
       </c>
       <c r="O6" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="P6" t="s">
         <v>36</v>
       </c>
-      <c r="Q6" s="17" t="s">
-        <v>133</v>
+      <c r="Q6" t="s">
+        <v>151</v>
       </c>
       <c r="R6" t="s">
         <v>42</v>
       </c>
-      <c r="S6">
-        <v>3.9E-2</v>
+      <c r="S6" t="s">
+        <v>152</v>
       </c>
       <c r="T6" t="s">
         <v>46</v>
@@ -1819,96 +1873,19 @@
       <c r="U6" t="s">
         <v>40</v>
       </c>
-      <c r="V6">
-        <v>49.875</v>
+      <c r="V6" t="s">
+        <v>153</v>
       </c>
       <c r="W6" t="s">
         <v>46</v>
       </c>
-      <c r="AF6">
-        <v>39150</v>
+      <c r="AF6" t="s">
+        <v>163</v>
       </c>
       <c r="AG6" t="s">
         <v>49</v>
       </c>
       <c r="AH6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C7" t="s">
-        <v>129</v>
-      </c>
-      <c r="D7" t="s">
-        <v>130</v>
-      </c>
-      <c r="E7" t="s">
-        <v>63</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>83</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7" t="s">
-        <v>38</v>
-      </c>
-      <c r="K7" t="s">
-        <v>144</v>
-      </c>
-      <c r="L7" t="s">
-        <v>57</v>
-      </c>
-      <c r="M7" t="s">
-        <v>145</v>
-      </c>
-      <c r="N7" t="s">
-        <v>37</v>
-      </c>
-      <c r="O7" t="s">
-        <v>137</v>
-      </c>
-      <c r="P7" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q7" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="R7" t="s">
-        <v>42</v>
-      </c>
-      <c r="S7">
-        <v>3.9E-2</v>
-      </c>
-      <c r="T7" t="s">
-        <v>46</v>
-      </c>
-      <c r="U7" t="s">
-        <v>40</v>
-      </c>
-      <c r="V7">
-        <v>49.875</v>
-      </c>
-      <c r="W7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AF7">
-        <v>38570</v>
-      </c>
-      <c r="AG7" t="s">
-        <v>49</v>
-      </c>
-      <c r="AH7" t="s">
         <v>132</v>
       </c>
     </row>
@@ -1926,7 +1903,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="12">
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{3A6724BF-6BD4-4C3F-81B8-5C31DA69CDFD}">
           <x14:formula1>
@@ -2016,14 +1993,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="9" customWidth="1"/>
-    <col min="5" max="5" width="30.42578125" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="7"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="12" max="12" width="18.28515625" customWidth="1"/>
-    <col min="14" max="14" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="25.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="9" width="12.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="30.42578125" collapsed="true"/>
+    <col min="6" max="6" style="7" width="9.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="18.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:23" ht="37.5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fix Multiple Bugs with Algoma Receptions Function
Fixed bug where Heidtman Butler order was not being found in the system.

Fixed bug where system would not wait until upload of import manifest is finished to close browser.

Fixed bug where multi-page releases were not being parsed and uploaded.
</commit_message>
<xml_diff>
--- a/Nasco-Database-Web-App/import-manifest.xlsx
+++ b/Nasco-Database-Web-App/import-manifest.xlsx
@@ -288,7 +288,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2192" uniqueCount="245">
   <si>
     <t xml:space="preserve">Client inventory </t>
   </si>
@@ -780,6 +780,249 @@
   </si>
   <si>
     <t>44,670</t>
+  </si>
+  <si>
+    <t>Esmark C/O CSI University Park - 19843</t>
+  </si>
+  <si>
+    <t>Hot Rolled Steel Sheet</t>
+  </si>
+  <si>
+    <t>PCY4495</t>
+  </si>
+  <si>
+    <t>2341J5 05</t>
+  </si>
+  <si>
+    <t>1200025017 / 2202011 / IH38407/8</t>
+  </si>
+  <si>
+    <t>0.0970</t>
+  </si>
+  <si>
+    <t>44,070</t>
+  </si>
+  <si>
+    <t>PCY4496</t>
+  </si>
+  <si>
+    <t>2341J5 55</t>
+  </si>
+  <si>
+    <t>44,230</t>
+  </si>
+  <si>
+    <t>PCY5461</t>
+  </si>
+  <si>
+    <t>2449J5 56</t>
+  </si>
+  <si>
+    <t>1200025017 / 2202011 / FH38603/6</t>
+  </si>
+  <si>
+    <t>0.1120</t>
+  </si>
+  <si>
+    <t>51.500</t>
+  </si>
+  <si>
+    <t>46,060</t>
+  </si>
+  <si>
+    <t>PCY5462</t>
+  </si>
+  <si>
+    <t>2450J5 01</t>
+  </si>
+  <si>
+    <t>41,860</t>
+  </si>
+  <si>
+    <t>Heidtman Butler IN - 46365</t>
+  </si>
+  <si>
+    <t>TCY3570</t>
+  </si>
+  <si>
+    <t>2246J5 54</t>
+  </si>
+  <si>
+    <t>1200024997 / 2201532 / HP83024-1-1/1</t>
+  </si>
+  <si>
+    <t>0.0368</t>
+  </si>
+  <si>
+    <t>58.010</t>
+  </si>
+  <si>
+    <t>36,530</t>
+  </si>
+  <si>
+    <t>TCX4091</t>
+  </si>
+  <si>
+    <t>1002J5 06</t>
+  </si>
+  <si>
+    <t>1200024997 / 2201532 / HP83025-1-1/1</t>
+  </si>
+  <si>
+    <t>0.0450</t>
+  </si>
+  <si>
+    <t>58.500</t>
+  </si>
+  <si>
+    <t>33,200</t>
+  </si>
+  <si>
+    <t>TCY8973</t>
+  </si>
+  <si>
+    <t>2885J5 04</t>
+  </si>
+  <si>
+    <t>1200024997 / 2201532 / HP83703-1-1/1</t>
+  </si>
+  <si>
+    <t>0.0710</t>
+  </si>
+  <si>
+    <t>51.375</t>
+  </si>
+  <si>
+    <t>43,190</t>
+  </si>
+  <si>
+    <t>TCY8974</t>
+  </si>
+  <si>
+    <t>2885J5 54</t>
+  </si>
+  <si>
+    <t>41,770</t>
+  </si>
+  <si>
+    <t>TCY8980</t>
+  </si>
+  <si>
+    <t>2886J5 52</t>
+  </si>
+  <si>
+    <t>43,180</t>
+  </si>
+  <si>
+    <t>TCY3839</t>
+  </si>
+  <si>
+    <t>2273J5 04</t>
+  </si>
+  <si>
+    <t>1200024963 / 2201532 / SP78826-1-1/1</t>
+  </si>
+  <si>
+    <t>0.0320</t>
+  </si>
+  <si>
+    <t>45,770</t>
+  </si>
+  <si>
+    <t>TCY3838</t>
+  </si>
+  <si>
+    <t>2273J5 53</t>
+  </si>
+  <si>
+    <t>44,190</t>
+  </si>
+  <si>
+    <t>TCY3832</t>
+  </si>
+  <si>
+    <t>2272J5 56</t>
+  </si>
+  <si>
+    <t>1200024963 / 2201532 / SP80409-1-1/1</t>
+  </si>
+  <si>
+    <t>0.1280</t>
+  </si>
+  <si>
+    <t>43,640</t>
+  </si>
+  <si>
+    <t>TCY3833</t>
+  </si>
+  <si>
+    <t>2273J5 01</t>
+  </si>
+  <si>
+    <t>44,680</t>
+  </si>
+  <si>
+    <t>Heidtman Butler IN - 48365</t>
+  </si>
+  <si>
+    <t>TCY3133</t>
+  </si>
+  <si>
+    <t>2187J5 04</t>
+  </si>
+  <si>
+    <t>1200024985 / 2201532 / SP75963-1-1/1</t>
+  </si>
+  <si>
+    <t>46,260</t>
+  </si>
+  <si>
+    <t>TCY3132</t>
+  </si>
+  <si>
+    <t>2187J5 53</t>
+  </si>
+  <si>
+    <t>44,490</t>
+  </si>
+  <si>
+    <t>Heidtman East Chicago, IN - 41941</t>
+  </si>
+  <si>
+    <t>SCX4406</t>
+  </si>
+  <si>
+    <t>1044J5 57</t>
+  </si>
+  <si>
+    <t>1200024985 / 2203067 / BX82791-1-1/1</t>
+  </si>
+  <si>
+    <t>0.0440</t>
+  </si>
+  <si>
+    <t>38.375</t>
+  </si>
+  <si>
+    <t>30,460</t>
+  </si>
+  <si>
+    <t>TCY0598</t>
+  </si>
+  <si>
+    <t>1855J5 57</t>
+  </si>
+  <si>
+    <t>34,550</t>
+  </si>
+  <si>
+    <t>TCY0599</t>
+  </si>
+  <si>
+    <t>1855J5 58</t>
+  </si>
+  <si>
+    <t>34,620</t>
   </si>
 </sst>
 </file>
@@ -1335,7 +1578,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E028D80B-E87B-4934-9799-6D8D159AC64A}">
-  <dimension ref="A1:AS6"/>
+  <dimension ref="A1:AS7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="T3" activePane="bottomRight" state="frozen"/>
@@ -1586,7 +1829,7 @@
         <v>131</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>224</v>
       </c>
       <c r="C3" t="s">
         <v>129</v>
@@ -1610,19 +1853,19 @@
         <v>38</v>
       </c>
       <c r="K3" t="s">
-        <v>148</v>
+        <v>225</v>
       </c>
       <c r="L3" t="s">
         <v>57</v>
       </c>
       <c r="M3" t="s">
-        <v>149</v>
+        <v>226</v>
       </c>
       <c r="N3" t="s">
         <v>37</v>
       </c>
       <c r="O3" t="s">
-        <v>150</v>
+        <v>227</v>
       </c>
       <c r="P3" t="s">
         <v>36</v>
@@ -1634,7 +1877,7 @@
         <v>42</v>
       </c>
       <c r="S3" t="s">
-        <v>152</v>
+        <v>193</v>
       </c>
       <c r="T3" t="s">
         <v>46</v>
@@ -1649,7 +1892,7 @@
         <v>46</v>
       </c>
       <c r="AF3" t="s">
-        <v>154</v>
+        <v>228</v>
       </c>
       <c r="AG3" t="s">
         <v>49</v>
@@ -1663,7 +1906,7 @@
         <v>131</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>224</v>
       </c>
       <c r="C4" t="s">
         <v>129</v>
@@ -1687,19 +1930,19 @@
         <v>38</v>
       </c>
       <c r="K4" t="s">
-        <v>155</v>
+        <v>229</v>
       </c>
       <c r="L4" t="s">
         <v>57</v>
       </c>
       <c r="M4" t="s">
-        <v>156</v>
+        <v>230</v>
       </c>
       <c r="N4" t="s">
         <v>37</v>
       </c>
       <c r="O4" t="s">
-        <v>150</v>
+        <v>227</v>
       </c>
       <c r="P4" t="s">
         <v>36</v>
@@ -1711,7 +1954,7 @@
         <v>42</v>
       </c>
       <c r="S4" t="s">
-        <v>152</v>
+        <v>193</v>
       </c>
       <c r="T4" t="s">
         <v>46</v>
@@ -1726,7 +1969,7 @@
         <v>46</v>
       </c>
       <c r="AF4" t="s">
-        <v>157</v>
+        <v>231</v>
       </c>
       <c r="AG4" t="s">
         <v>49</v>
@@ -1740,7 +1983,7 @@
         <v>131</v>
       </c>
       <c r="B5" t="s">
-        <v>146</v>
+        <v>232</v>
       </c>
       <c r="C5" t="s">
         <v>129</v>
@@ -1764,19 +2007,19 @@
         <v>38</v>
       </c>
       <c r="K5" t="s">
-        <v>158</v>
+        <v>233</v>
       </c>
       <c r="L5" t="s">
         <v>57</v>
       </c>
       <c r="M5" t="s">
-        <v>159</v>
+        <v>234</v>
       </c>
       <c r="N5" t="s">
         <v>37</v>
       </c>
       <c r="O5" t="s">
-        <v>150</v>
+        <v>235</v>
       </c>
       <c r="P5" t="s">
         <v>36</v>
@@ -1788,7 +2031,7 @@
         <v>42</v>
       </c>
       <c r="S5" t="s">
-        <v>152</v>
+        <v>236</v>
       </c>
       <c r="T5" t="s">
         <v>46</v>
@@ -1797,13 +2040,13 @@
         <v>40</v>
       </c>
       <c r="V5" t="s">
-        <v>153</v>
+        <v>237</v>
       </c>
       <c r="W5" t="s">
         <v>46</v>
       </c>
       <c r="AF5" t="s">
-        <v>160</v>
+        <v>238</v>
       </c>
       <c r="AG5" t="s">
         <v>49</v>
@@ -1817,7 +2060,7 @@
         <v>131</v>
       </c>
       <c r="B6" t="s">
-        <v>146</v>
+        <v>232</v>
       </c>
       <c r="C6" t="s">
         <v>129</v>
@@ -1841,19 +2084,19 @@
         <v>38</v>
       </c>
       <c r="K6" t="s">
-        <v>161</v>
+        <v>239</v>
       </c>
       <c r="L6" t="s">
         <v>57</v>
       </c>
       <c r="M6" t="s">
-        <v>162</v>
+        <v>240</v>
       </c>
       <c r="N6" t="s">
         <v>37</v>
       </c>
       <c r="O6" t="s">
-        <v>150</v>
+        <v>235</v>
       </c>
       <c r="P6" t="s">
         <v>36</v>
@@ -1865,7 +2108,7 @@
         <v>42</v>
       </c>
       <c r="S6" t="s">
-        <v>152</v>
+        <v>236</v>
       </c>
       <c r="T6" t="s">
         <v>46</v>
@@ -1874,18 +2117,95 @@
         <v>40</v>
       </c>
       <c r="V6" t="s">
-        <v>153</v>
+        <v>237</v>
       </c>
       <c r="W6" t="s">
         <v>46</v>
       </c>
       <c r="AF6" t="s">
-        <v>163</v>
+        <v>241</v>
       </c>
       <c r="AG6" t="s">
         <v>49</v>
       </c>
       <c r="AH6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" t="s">
+        <v>232</v>
+      </c>
+      <c r="C7" t="s">
+        <v>129</v>
+      </c>
+      <c r="D7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" t="s">
+        <v>147</v>
+      </c>
+      <c r="G7" t="s">
+        <v>83</v>
+      </c>
+      <c r="I7" t="s">
+        <v>147</v>
+      </c>
+      <c r="J7" t="s">
+        <v>38</v>
+      </c>
+      <c r="K7" t="s">
+        <v>242</v>
+      </c>
+      <c r="L7" t="s">
+        <v>57</v>
+      </c>
+      <c r="M7" t="s">
+        <v>243</v>
+      </c>
+      <c r="N7" t="s">
+        <v>37</v>
+      </c>
+      <c r="O7" t="s">
+        <v>235</v>
+      </c>
+      <c r="P7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>151</v>
+      </c>
+      <c r="R7" t="s">
+        <v>42</v>
+      </c>
+      <c r="S7" t="s">
+        <v>236</v>
+      </c>
+      <c r="T7" t="s">
+        <v>46</v>
+      </c>
+      <c r="U7" t="s">
+        <v>40</v>
+      </c>
+      <c r="V7" t="s">
+        <v>237</v>
+      </c>
+      <c r="W7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>244</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH7" t="s">
         <v>132</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Fields to current_inventory Table
Added fields necessary for implementation of reception logic to current_inventory table of MySql server.
</commit_message>
<xml_diff>
--- a/Nasco-Database-Web-App/import-manifest.xlsx
+++ b/Nasco-Database-Web-App/import-manifest.xlsx
@@ -288,7 +288,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2192" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2917" uniqueCount="332">
   <si>
     <t xml:space="preserve">Client inventory </t>
   </si>
@@ -1023,6 +1023,267 @@
   </si>
   <si>
     <t>34,620</t>
+  </si>
+  <si>
+    <t>Wheatland Tube, LLC - 74629</t>
+  </si>
+  <si>
+    <t>TCY6882</t>
+  </si>
+  <si>
+    <t>2634J5 04</t>
+  </si>
+  <si>
+    <t>1200025023 / 2202902 / 4500292059/1</t>
+  </si>
+  <si>
+    <t>0.0390</t>
+  </si>
+  <si>
+    <t>49.875</t>
+  </si>
+  <si>
+    <t>47,570</t>
+  </si>
+  <si>
+    <t>TCY6881</t>
+  </si>
+  <si>
+    <t>2634J5 54</t>
+  </si>
+  <si>
+    <t>46,500</t>
+  </si>
+  <si>
+    <t>TCY6888</t>
+  </si>
+  <si>
+    <t>2635J5 02</t>
+  </si>
+  <si>
+    <t>47,430</t>
+  </si>
+  <si>
+    <t>TCY6898</t>
+  </si>
+  <si>
+    <t>2636J5 02</t>
+  </si>
+  <si>
+    <t>47,410</t>
+  </si>
+  <si>
+    <t>TCY3134</t>
+  </si>
+  <si>
+    <t>2187J5 54</t>
+  </si>
+  <si>
+    <t>1200025027 / 2201532 / SP75963-1-1/1</t>
+  </si>
+  <si>
+    <t>44,090</t>
+  </si>
+  <si>
+    <t>SCY6889</t>
+  </si>
+  <si>
+    <t>2635J5 52</t>
+  </si>
+  <si>
+    <t>1200025027 / 2202902 / 4500292059/1</t>
+  </si>
+  <si>
+    <t>45,050</t>
+  </si>
+  <si>
+    <t>TCY6891</t>
+  </si>
+  <si>
+    <t>2635J5 53</t>
+  </si>
+  <si>
+    <t>46,370</t>
+  </si>
+  <si>
+    <t>TCY3116</t>
+  </si>
+  <si>
+    <t>2185J5 55</t>
+  </si>
+  <si>
+    <t>1200025027 / 2203067 / BX81403-1-1/1</t>
+  </si>
+  <si>
+    <t>0.0760</t>
+  </si>
+  <si>
+    <t>TCY6895</t>
+  </si>
+  <si>
+    <t>2635J5 55</t>
+  </si>
+  <si>
+    <t>1200025028 / 2202902 / 4500292059/1</t>
+  </si>
+  <si>
+    <t>46,340</t>
+  </si>
+  <si>
+    <t>TCY6899</t>
+  </si>
+  <si>
+    <t>2636J5 52</t>
+  </si>
+  <si>
+    <t>46,120</t>
+  </si>
+  <si>
+    <t>TCY6905</t>
+  </si>
+  <si>
+    <t>2636J5 55</t>
+  </si>
+  <si>
+    <t>46,290</t>
+  </si>
+  <si>
+    <t>TCY6860</t>
+  </si>
+  <si>
+    <t>2632J5 03</t>
+  </si>
+  <si>
+    <t>1200025028 / 2202902 / 4500292059/2</t>
+  </si>
+  <si>
+    <t>49.910</t>
+  </si>
+  <si>
+    <t>43,270</t>
+  </si>
+  <si>
+    <t>TCY6876</t>
+  </si>
+  <si>
+    <t>2634J5 01</t>
+  </si>
+  <si>
+    <t>1200025041 / 2202902 / 4500292059/1</t>
+  </si>
+  <si>
+    <t>47,830</t>
+  </si>
+  <si>
+    <t>TCY6878</t>
+  </si>
+  <si>
+    <t>2634J5 02</t>
+  </si>
+  <si>
+    <t>SCY6892</t>
+  </si>
+  <si>
+    <t>2635J5 04</t>
+  </si>
+  <si>
+    <t>46,390</t>
+  </si>
+  <si>
+    <t>TCY6904</t>
+  </si>
+  <si>
+    <t>2636J5 05</t>
+  </si>
+  <si>
+    <t>47,140</t>
+  </si>
+  <si>
+    <t>TCY4181</t>
+  </si>
+  <si>
+    <t>2308J5 04</t>
+  </si>
+  <si>
+    <t>1200025050 / 2202011 / IC37835/1</t>
+  </si>
+  <si>
+    <t>44,480</t>
+  </si>
+  <si>
+    <t>TCY4183</t>
+  </si>
+  <si>
+    <t>2308J5 05</t>
+  </si>
+  <si>
+    <t>44,260</t>
+  </si>
+  <si>
+    <t>TCY4182</t>
+  </si>
+  <si>
+    <t>2308J5 54</t>
+  </si>
+  <si>
+    <t>42,980</t>
+  </si>
+  <si>
+    <t>TCY4185</t>
+  </si>
+  <si>
+    <t>2309J5 01</t>
+  </si>
+  <si>
+    <t>44,600</t>
+  </si>
+  <si>
+    <t>Steel Warehouse - 93158</t>
+  </si>
+  <si>
+    <t>TCY8024</t>
+  </si>
+  <si>
+    <t>2759J5 02</t>
+  </si>
+  <si>
+    <t>1200025024 / 2203158 / L02524/1</t>
+  </si>
+  <si>
+    <t>0.0580</t>
+  </si>
+  <si>
+    <t>48.500</t>
+  </si>
+  <si>
+    <t>45,200</t>
+  </si>
+  <si>
+    <t>TCY8026</t>
+  </si>
+  <si>
+    <t>2759J5 03</t>
+  </si>
+  <si>
+    <t>46,220</t>
+  </si>
+  <si>
+    <t>TCY8025</t>
+  </si>
+  <si>
+    <t>2759J5 52</t>
+  </si>
+  <si>
+    <t>44,860</t>
+  </si>
+  <si>
+    <t>TCY8027</t>
+  </si>
+  <si>
+    <t>2759J5 53</t>
+  </si>
+  <si>
+    <t>43,820</t>
   </si>
 </sst>
 </file>
@@ -1578,7 +1839,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E028D80B-E87B-4934-9799-6D8D159AC64A}">
-  <dimension ref="A1:AS7"/>
+  <dimension ref="A1:AS6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="T3" activePane="bottomRight" state="frozen"/>
@@ -1829,13 +2090,13 @@
         <v>131</v>
       </c>
       <c r="B3" t="s">
-        <v>224</v>
+        <v>316</v>
       </c>
       <c r="C3" t="s">
         <v>129</v>
       </c>
       <c r="D3" t="s">
-        <v>130</v>
+        <v>165</v>
       </c>
       <c r="E3" t="s">
         <v>63</v>
@@ -1853,19 +2114,19 @@
         <v>38</v>
       </c>
       <c r="K3" t="s">
-        <v>225</v>
+        <v>317</v>
       </c>
       <c r="L3" t="s">
         <v>57</v>
       </c>
       <c r="M3" t="s">
-        <v>226</v>
+        <v>318</v>
       </c>
       <c r="N3" t="s">
         <v>37</v>
       </c>
       <c r="O3" t="s">
-        <v>227</v>
+        <v>319</v>
       </c>
       <c r="P3" t="s">
         <v>36</v>
@@ -1877,7 +2138,7 @@
         <v>42</v>
       </c>
       <c r="S3" t="s">
-        <v>193</v>
+        <v>320</v>
       </c>
       <c r="T3" t="s">
         <v>46</v>
@@ -1886,13 +2147,13 @@
         <v>40</v>
       </c>
       <c r="V3" t="s">
-        <v>153</v>
+        <v>321</v>
       </c>
       <c r="W3" t="s">
         <v>46</v>
       </c>
       <c r="AF3" t="s">
-        <v>228</v>
+        <v>322</v>
       </c>
       <c r="AG3" t="s">
         <v>49</v>
@@ -1906,13 +2167,13 @@
         <v>131</v>
       </c>
       <c r="B4" t="s">
-        <v>224</v>
+        <v>316</v>
       </c>
       <c r="C4" t="s">
         <v>129</v>
       </c>
       <c r="D4" t="s">
-        <v>130</v>
+        <v>165</v>
       </c>
       <c r="E4" t="s">
         <v>63</v>
@@ -1930,19 +2191,19 @@
         <v>38</v>
       </c>
       <c r="K4" t="s">
-        <v>229</v>
+        <v>323</v>
       </c>
       <c r="L4" t="s">
         <v>57</v>
       </c>
       <c r="M4" t="s">
-        <v>230</v>
+        <v>324</v>
       </c>
       <c r="N4" t="s">
         <v>37</v>
       </c>
       <c r="O4" t="s">
-        <v>227</v>
+        <v>319</v>
       </c>
       <c r="P4" t="s">
         <v>36</v>
@@ -1954,7 +2215,7 @@
         <v>42</v>
       </c>
       <c r="S4" t="s">
-        <v>193</v>
+        <v>320</v>
       </c>
       <c r="T4" t="s">
         <v>46</v>
@@ -1963,13 +2224,13 @@
         <v>40</v>
       </c>
       <c r="V4" t="s">
-        <v>153</v>
+        <v>321</v>
       </c>
       <c r="W4" t="s">
         <v>46</v>
       </c>
       <c r="AF4" t="s">
-        <v>231</v>
+        <v>325</v>
       </c>
       <c r="AG4" t="s">
         <v>49</v>
@@ -1983,13 +2244,13 @@
         <v>131</v>
       </c>
       <c r="B5" t="s">
-        <v>232</v>
+        <v>316</v>
       </c>
       <c r="C5" t="s">
         <v>129</v>
       </c>
       <c r="D5" t="s">
-        <v>130</v>
+        <v>165</v>
       </c>
       <c r="E5" t="s">
         <v>63</v>
@@ -2007,19 +2268,19 @@
         <v>38</v>
       </c>
       <c r="K5" t="s">
-        <v>233</v>
+        <v>326</v>
       </c>
       <c r="L5" t="s">
         <v>57</v>
       </c>
       <c r="M5" t="s">
-        <v>234</v>
+        <v>327</v>
       </c>
       <c r="N5" t="s">
         <v>37</v>
       </c>
       <c r="O5" t="s">
-        <v>235</v>
+        <v>319</v>
       </c>
       <c r="P5" t="s">
         <v>36</v>
@@ -2031,7 +2292,7 @@
         <v>42</v>
       </c>
       <c r="S5" t="s">
-        <v>236</v>
+        <v>320</v>
       </c>
       <c r="T5" t="s">
         <v>46</v>
@@ -2040,13 +2301,13 @@
         <v>40</v>
       </c>
       <c r="V5" t="s">
-        <v>237</v>
+        <v>321</v>
       </c>
       <c r="W5" t="s">
         <v>46</v>
       </c>
       <c r="AF5" t="s">
-        <v>238</v>
+        <v>328</v>
       </c>
       <c r="AG5" t="s">
         <v>49</v>
@@ -2060,13 +2321,13 @@
         <v>131</v>
       </c>
       <c r="B6" t="s">
-        <v>232</v>
+        <v>316</v>
       </c>
       <c r="C6" t="s">
         <v>129</v>
       </c>
       <c r="D6" t="s">
-        <v>130</v>
+        <v>165</v>
       </c>
       <c r="E6" t="s">
         <v>63</v>
@@ -2084,19 +2345,19 @@
         <v>38</v>
       </c>
       <c r="K6" t="s">
-        <v>239</v>
+        <v>329</v>
       </c>
       <c r="L6" t="s">
         <v>57</v>
       </c>
       <c r="M6" t="s">
-        <v>240</v>
+        <v>330</v>
       </c>
       <c r="N6" t="s">
         <v>37</v>
       </c>
       <c r="O6" t="s">
-        <v>235</v>
+        <v>319</v>
       </c>
       <c r="P6" t="s">
         <v>36</v>
@@ -2108,7 +2369,7 @@
         <v>42</v>
       </c>
       <c r="S6" t="s">
-        <v>236</v>
+        <v>320</v>
       </c>
       <c r="T6" t="s">
         <v>46</v>
@@ -2117,95 +2378,18 @@
         <v>40</v>
       </c>
       <c r="V6" t="s">
-        <v>237</v>
+        <v>321</v>
       </c>
       <c r="W6" t="s">
         <v>46</v>
       </c>
       <c r="AF6" t="s">
-        <v>241</v>
+        <v>331</v>
       </c>
       <c r="AG6" t="s">
         <v>49</v>
       </c>
       <c r="AH6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B7" t="s">
-        <v>232</v>
-      </c>
-      <c r="C7" t="s">
-        <v>129</v>
-      </c>
-      <c r="D7" t="s">
-        <v>130</v>
-      </c>
-      <c r="E7" t="s">
-        <v>63</v>
-      </c>
-      <c r="F7" t="s">
-        <v>147</v>
-      </c>
-      <c r="G7" t="s">
-        <v>83</v>
-      </c>
-      <c r="I7" t="s">
-        <v>147</v>
-      </c>
-      <c r="J7" t="s">
-        <v>38</v>
-      </c>
-      <c r="K7" t="s">
-        <v>242</v>
-      </c>
-      <c r="L7" t="s">
-        <v>57</v>
-      </c>
-      <c r="M7" t="s">
-        <v>243</v>
-      </c>
-      <c r="N7" t="s">
-        <v>37</v>
-      </c>
-      <c r="O7" t="s">
-        <v>235</v>
-      </c>
-      <c r="P7" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>151</v>
-      </c>
-      <c r="R7" t="s">
-        <v>42</v>
-      </c>
-      <c r="S7" t="s">
-        <v>236</v>
-      </c>
-      <c r="T7" t="s">
-        <v>46</v>
-      </c>
-      <c r="U7" t="s">
-        <v>40</v>
-      </c>
-      <c r="V7" t="s">
-        <v>237</v>
-      </c>
-      <c r="W7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>244</v>
-      </c>
-      <c r="AG7" t="s">
-        <v>49</v>
-      </c>
-      <c r="AH7" t="s">
         <v>132</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update IDs for Browser Automation
Updated IDs for Browser Automation and attempted to fix chromedriver errors when using with Heroku
</commit_message>
<xml_diff>
--- a/Nasco-Database-Web-App/import-manifest.xlsx
+++ b/Nasco-Database-Web-App/import-manifest.xlsx
@@ -288,7 +288,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2917" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3313" uniqueCount="400">
   <si>
     <t xml:space="preserve">Client inventory </t>
   </si>
@@ -1284,6 +1284,210 @@
   </si>
   <si>
     <t>43,820</t>
+  </si>
+  <si>
+    <t>SCZ8245</t>
+  </si>
+  <si>
+    <t>4147J5 05</t>
+  </si>
+  <si>
+    <t>1200025327 / 2202011 / FH38737/2</t>
+  </si>
+  <si>
+    <t>12/08/21</t>
+  </si>
+  <si>
+    <t>60.000</t>
+  </si>
+  <si>
+    <t>45,990</t>
+  </si>
+  <si>
+    <t>TCZ8244</t>
+  </si>
+  <si>
+    <t>4147J5 55</t>
+  </si>
+  <si>
+    <t>45,980</t>
+  </si>
+  <si>
+    <t>TCZ8247</t>
+  </si>
+  <si>
+    <t>4148J5 01</t>
+  </si>
+  <si>
+    <t>41,960</t>
+  </si>
+  <si>
+    <t>TCZ8249</t>
+  </si>
+  <si>
+    <t>4148J5 02</t>
+  </si>
+  <si>
+    <t>46,090</t>
+  </si>
+  <si>
+    <t>HDA1903</t>
+  </si>
+  <si>
+    <t>4605J5 05</t>
+  </si>
+  <si>
+    <t>1200025362 / 2201532 / HP84663-1-1/1</t>
+  </si>
+  <si>
+    <t>0.3680</t>
+  </si>
+  <si>
+    <t>50.750</t>
+  </si>
+  <si>
+    <t>46,980</t>
+  </si>
+  <si>
+    <t>HDA1904</t>
+  </si>
+  <si>
+    <t>4605J5 55</t>
+  </si>
+  <si>
+    <t>47,233</t>
+  </si>
+  <si>
+    <t>HR FLOOR PLATE</t>
+  </si>
+  <si>
+    <t>HCZ8465</t>
+  </si>
+  <si>
+    <t>4170J5 54</t>
+  </si>
+  <si>
+    <t>1200025362 / 2202011 / FH39108/4</t>
+  </si>
+  <si>
+    <t>0.1780</t>
+  </si>
+  <si>
+    <t>61.000</t>
+  </si>
+  <si>
+    <t>35,053</t>
+  </si>
+  <si>
+    <t>Esmark C/O Ratner Steel - 12850</t>
+  </si>
+  <si>
+    <t>LCZ8218</t>
+  </si>
+  <si>
+    <t>4145J5 01</t>
+  </si>
+  <si>
+    <t>1200025362 / 2203302 / FH38601/1</t>
+  </si>
+  <si>
+    <t>0.2400</t>
+  </si>
+  <si>
+    <t>36,160</t>
+  </si>
+  <si>
+    <t>TCZ8250</t>
+  </si>
+  <si>
+    <t>4148J5 03</t>
+  </si>
+  <si>
+    <t>1200025316 / 2202011 / FH38737/2</t>
+  </si>
+  <si>
+    <t>46,150</t>
+  </si>
+  <si>
+    <t>TCZ8246</t>
+  </si>
+  <si>
+    <t>4148J5 51</t>
+  </si>
+  <si>
+    <t>46,080</t>
+  </si>
+  <si>
+    <t>SCZ7150</t>
+  </si>
+  <si>
+    <t>4014J5 05</t>
+  </si>
+  <si>
+    <t>1200025316 / 2202011 / FH38736/2</t>
+  </si>
+  <si>
+    <t>0.1700</t>
+  </si>
+  <si>
+    <t>46,200</t>
+  </si>
+  <si>
+    <t>SCZ7146</t>
+  </si>
+  <si>
+    <t>4014J5 53</t>
+  </si>
+  <si>
+    <t>45,730</t>
+  </si>
+  <si>
+    <t>Hot Rolled Coils</t>
+  </si>
+  <si>
+    <t>XCZ9287</t>
+  </si>
+  <si>
+    <t>4277J5 05</t>
+  </si>
+  <si>
+    <t>1200025324 /  / 506267/8</t>
+  </si>
+  <si>
+    <t>0.1805</t>
+  </si>
+  <si>
+    <t>52.890</t>
+  </si>
+  <si>
+    <t>46,203</t>
+  </si>
+  <si>
+    <t>XCZ9290</t>
+  </si>
+  <si>
+    <t>4278J5 01</t>
+  </si>
+  <si>
+    <t>45,861</t>
+  </si>
+  <si>
+    <t>XCZ9291</t>
+  </si>
+  <si>
+    <t>4278J5 51</t>
+  </si>
+  <si>
+    <t>46,343</t>
+  </si>
+  <si>
+    <t>XCZ9300</t>
+  </si>
+  <si>
+    <t>4279J5 01</t>
+  </si>
+  <si>
+    <t>45,784</t>
   </si>
 </sst>
 </file>
@@ -2089,14 +2293,12 @@
       <c r="A3" t="s">
         <v>131</v>
       </c>
-      <c r="B3" t="s">
-        <v>316</v>
-      </c>
+      <c r="B3"/>
       <c r="C3" t="s">
         <v>129</v>
       </c>
       <c r="D3" t="s">
-        <v>165</v>
+        <v>384</v>
       </c>
       <c r="E3" t="s">
         <v>63</v>
@@ -2114,31 +2316,31 @@
         <v>38</v>
       </c>
       <c r="K3" t="s">
-        <v>317</v>
+        <v>385</v>
       </c>
       <c r="L3" t="s">
         <v>57</v>
       </c>
       <c r="M3" t="s">
-        <v>318</v>
+        <v>386</v>
       </c>
       <c r="N3" t="s">
         <v>37</v>
       </c>
       <c r="O3" t="s">
-        <v>319</v>
+        <v>387</v>
       </c>
       <c r="P3" t="s">
         <v>36</v>
       </c>
       <c r="Q3" t="s">
-        <v>151</v>
+        <v>335</v>
       </c>
       <c r="R3" t="s">
         <v>42</v>
       </c>
       <c r="S3" t="s">
-        <v>320</v>
+        <v>388</v>
       </c>
       <c r="T3" t="s">
         <v>46</v>
@@ -2147,13 +2349,13 @@
         <v>40</v>
       </c>
       <c r="V3" t="s">
-        <v>321</v>
+        <v>389</v>
       </c>
       <c r="W3" t="s">
         <v>46</v>
       </c>
       <c r="AF3" t="s">
-        <v>322</v>
+        <v>390</v>
       </c>
       <c r="AG3" t="s">
         <v>49</v>
@@ -2166,14 +2368,12 @@
       <c r="A4" t="s">
         <v>131</v>
       </c>
-      <c r="B4" t="s">
-        <v>316</v>
-      </c>
+      <c r="B4"/>
       <c r="C4" t="s">
         <v>129</v>
       </c>
       <c r="D4" t="s">
-        <v>165</v>
+        <v>384</v>
       </c>
       <c r="E4" t="s">
         <v>63</v>
@@ -2191,31 +2391,31 @@
         <v>38</v>
       </c>
       <c r="K4" t="s">
-        <v>323</v>
+        <v>391</v>
       </c>
       <c r="L4" t="s">
         <v>57</v>
       </c>
       <c r="M4" t="s">
-        <v>324</v>
+        <v>392</v>
       </c>
       <c r="N4" t="s">
         <v>37</v>
       </c>
       <c r="O4" t="s">
-        <v>319</v>
+        <v>387</v>
       </c>
       <c r="P4" t="s">
         <v>36</v>
       </c>
       <c r="Q4" t="s">
-        <v>151</v>
+        <v>335</v>
       </c>
       <c r="R4" t="s">
         <v>42</v>
       </c>
       <c r="S4" t="s">
-        <v>320</v>
+        <v>388</v>
       </c>
       <c r="T4" t="s">
         <v>46</v>
@@ -2224,13 +2424,13 @@
         <v>40</v>
       </c>
       <c r="V4" t="s">
-        <v>321</v>
+        <v>389</v>
       </c>
       <c r="W4" t="s">
         <v>46</v>
       </c>
       <c r="AF4" t="s">
-        <v>325</v>
+        <v>393</v>
       </c>
       <c r="AG4" t="s">
         <v>49</v>
@@ -2243,14 +2443,12 @@
       <c r="A5" t="s">
         <v>131</v>
       </c>
-      <c r="B5" t="s">
-        <v>316</v>
-      </c>
+      <c r="B5"/>
       <c r="C5" t="s">
         <v>129</v>
       </c>
       <c r="D5" t="s">
-        <v>165</v>
+        <v>384</v>
       </c>
       <c r="E5" t="s">
         <v>63</v>
@@ -2268,31 +2466,31 @@
         <v>38</v>
       </c>
       <c r="K5" t="s">
-        <v>326</v>
+        <v>394</v>
       </c>
       <c r="L5" t="s">
         <v>57</v>
       </c>
       <c r="M5" t="s">
-        <v>327</v>
+        <v>395</v>
       </c>
       <c r="N5" t="s">
         <v>37</v>
       </c>
       <c r="O5" t="s">
-        <v>319</v>
+        <v>387</v>
       </c>
       <c r="P5" t="s">
         <v>36</v>
       </c>
       <c r="Q5" t="s">
-        <v>151</v>
+        <v>335</v>
       </c>
       <c r="R5" t="s">
         <v>42</v>
       </c>
       <c r="S5" t="s">
-        <v>320</v>
+        <v>388</v>
       </c>
       <c r="T5" t="s">
         <v>46</v>
@@ -2301,13 +2499,13 @@
         <v>40</v>
       </c>
       <c r="V5" t="s">
-        <v>321</v>
+        <v>389</v>
       </c>
       <c r="W5" t="s">
         <v>46</v>
       </c>
       <c r="AF5" t="s">
-        <v>328</v>
+        <v>396</v>
       </c>
       <c r="AG5" t="s">
         <v>49</v>
@@ -2320,14 +2518,12 @@
       <c r="A6" t="s">
         <v>131</v>
       </c>
-      <c r="B6" t="s">
-        <v>316</v>
-      </c>
+      <c r="B6"/>
       <c r="C6" t="s">
         <v>129</v>
       </c>
       <c r="D6" t="s">
-        <v>165</v>
+        <v>384</v>
       </c>
       <c r="E6" t="s">
         <v>63</v>
@@ -2345,31 +2541,31 @@
         <v>38</v>
       </c>
       <c r="K6" t="s">
-        <v>329</v>
+        <v>397</v>
       </c>
       <c r="L6" t="s">
         <v>57</v>
       </c>
       <c r="M6" t="s">
-        <v>330</v>
+        <v>398</v>
       </c>
       <c r="N6" t="s">
         <v>37</v>
       </c>
       <c r="O6" t="s">
-        <v>319</v>
+        <v>387</v>
       </c>
       <c r="P6" t="s">
         <v>36</v>
       </c>
       <c r="Q6" t="s">
-        <v>151</v>
+        <v>335</v>
       </c>
       <c r="R6" t="s">
         <v>42</v>
       </c>
       <c r="S6" t="s">
-        <v>320</v>
+        <v>388</v>
       </c>
       <c r="T6" t="s">
         <v>46</v>
@@ -2378,13 +2574,13 @@
         <v>40</v>
       </c>
       <c r="V6" t="s">
-        <v>321</v>
+        <v>389</v>
       </c>
       <c r="W6" t="s">
         <v>46</v>
       </c>
       <c r="AF6" t="s">
-        <v>331</v>
+        <v>399</v>
       </c>
       <c r="AG6" t="s">
         <v>49</v>

</xml_diff>